<commit_message>
Adding readme file to directory.  This file describes the steps to run the generic model for an attached house.
minor change to .choice and .options file to allow for the roof height (calculated based on roof slope) to be included. This required a new tag in the roof.geo file.
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-3storey/3storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-3storey/3storey_model_geometry.xlsx
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
   <si>
     <t>window geometry calculations</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>8/12</t>
+  </si>
+  <si>
+    <t>3/12</t>
   </si>
 </sst>
 </file>
@@ -747,7 +750,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +759,7 @@
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -785,7 +788,7 @@
       </c>
       <c r="C2" s="13">
         <f>+C3*C4</f>
-        <v>98.399999999999991</v>
+        <v>198</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>4</v>
@@ -798,7 +801,7 @@
       </c>
       <c r="H2">
         <f>+(B24-B23)*(D29-D24)</f>
-        <v>36.575999999999993</v>
+        <v>50.291999999999994</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
@@ -812,7 +815,7 @@
         <v>76</v>
       </c>
       <c r="C3" s="2">
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -825,7 +828,7 @@
       </c>
       <c r="H3">
         <f>+(C25-C24)*(D29-D25)</f>
-        <v>24.993599999999994</v>
+        <v>36.575999999999993</v>
       </c>
       <c r="I3" t="s">
         <v>4</v>
@@ -839,7 +842,7 @@
         <v>77</v>
       </c>
       <c r="C4" s="1">
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -853,7 +856,7 @@
       </c>
       <c r="H4">
         <f>+(B25-B26)*(D29-D26)</f>
-        <v>36.575999999999993</v>
+        <v>50.291999999999994</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -878,7 +881,7 @@
       </c>
       <c r="H5">
         <f>+(C26-C23)*(D30-D26)</f>
-        <v>24.993599999999994</v>
+        <v>36.575999999999993</v>
       </c>
       <c r="I5" t="s">
         <v>4</v>
@@ -905,7 +908,7 @@
       </c>
       <c r="H6">
         <f>+(B28*C29)</f>
-        <v>98.399999999999991</v>
+        <v>198</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
@@ -930,7 +933,7 @@
       </c>
       <c r="H7">
         <f>+C26*B25</f>
-        <v>98.399999999999991</v>
+        <v>198</v>
       </c>
       <c r="I7" t="s">
         <v>4</v>
@@ -964,14 +967,14 @@
       </c>
       <c r="H8" s="15">
         <f>+H2*$C$5/100</f>
-        <v>5.4863999999999988</v>
+        <v>7.5437999999999992</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="19">
         <f>+H8/K8</f>
-        <v>3.5999999999999996</v>
+        <v>4.95</v>
       </c>
       <c r="K8" s="9">
         <f>+($C$8-$C$6)/2</f>
@@ -980,12 +983,12 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" t="s">
+      <c r="B9" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="13">
         <f>+C3/2</f>
-        <v>6</v>
+        <v>8.25</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>7</v>
@@ -998,14 +1001,14 @@
       </c>
       <c r="H9" s="16">
         <f>+H3*$C$5/100</f>
-        <v>3.749039999999999</v>
+        <v>5.4863999999999988</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="20">
         <f t="shared" ref="J9" si="0">+H9/K9</f>
-        <v>2.4599999999999995</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="K9" s="11">
         <f>+($C$8-$C$6)/2</f>
@@ -1028,14 +1031,14 @@
       </c>
       <c r="H10" s="17">
         <f>+H4*$C$5/100</f>
-        <v>5.4863999999999988</v>
+        <v>7.5437999999999992</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="21">
         <f>+H10/K10</f>
-        <v>3.5999999999999996</v>
+        <v>4.95</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" ref="K10:K11" si="1">+($C$8-$C$6)/2</f>
@@ -1060,14 +1063,14 @@
       </c>
       <c r="H11" s="18">
         <f>+H5*$C$5/100</f>
-        <v>3.749039999999999</v>
+        <v>5.4863999999999988</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="22">
         <f>+H11/K11</f>
-        <v>2.4599999999999995</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="K11" s="14">
         <f t="shared" si="1"/>
@@ -1092,7 +1095,7 @@
       </c>
       <c r="C13" s="15">
         <f>+$B$32</f>
-        <v>4.0999999999999996</v>
+        <v>5.45</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -1127,10 +1130,21 @@
       </c>
       <c r="C15" s="16">
         <f>+$C$36</f>
-        <v>2.9599999999999995</v>
-      </c>
-      <c r="G15" s="25"/>
-      <c r="H15" s="24"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="23">
+        <f>10.363+($C$3*H14)</f>
+        <v>21.363</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -1138,47 +1152,60 @@
       </c>
       <c r="C16" s="17">
         <f>+$B$39</f>
-        <v>11.5</v>
-      </c>
-      <c r="F16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H16" s="23">
-        <f>C8+(C3*H14)</f>
-        <v>13.4864</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>71</v>
       </c>
       <c r="C17" s="17">
         <f>+$B$40</f>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11.05</v>
+      </c>
+      <c r="F17" t="s">
+        <v>80</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="24">
+        <f>3/12</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="12">
         <f>+$C$43</f>
-        <v>7.6999999999999993</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11.5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>82</v>
+      </c>
+      <c r="H18" s="23">
+        <f>10.363+($C$3*H17)</f>
+        <v>14.488</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>73</v>
       </c>
       <c r="C19" s="18">
         <f>+$C$44</f>
-        <v>5.24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>61</v>
       </c>
@@ -1192,7 +1219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1207,13 +1234,13 @@
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>14</v>
       </c>
       <c r="B24" s="4">
         <f>+$C$3</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C24" s="3">
         <v>0</v>
@@ -1223,24 +1250,24 @@
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="4">
         <f>+$C$3</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C25" s="3">
         <f>+$C$4</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D25" s="3">
         <f>+$C$6</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1249,14 +1276,14 @@
       </c>
       <c r="C26" s="3">
         <f>+$C$4</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D26" s="3">
         <f>+$C$6</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1271,13 +1298,13 @@
         <v>5.4863999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="4">
         <f>+$C$3</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C28" s="3">
         <v>0</v>
@@ -1287,24 +1314,24 @@
         <v>5.4863999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
       <c r="B29" s="4">
         <f>+$C$3</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C29" s="3">
         <f>+$C$4</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D29" s="3">
         <f t="shared" si="2"/>
         <v>5.4863999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1313,14 +1340,14 @@
       </c>
       <c r="C30" s="3">
         <f>+$C$4</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D30" s="3">
         <f>+$C$8</f>
         <v>5.4863999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>21</v>
       </c>
@@ -1337,13 +1364,13 @@
         <v>2.9384000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B32" s="19">
         <f>+B31+$J$8</f>
-        <v>4.0999999999999996</v>
+        <v>5.45</v>
       </c>
       <c r="C32" s="9">
         <f>+C24</f>
@@ -1360,7 +1387,7 @@
       </c>
       <c r="B33" s="19">
         <f>+B31+$J$8</f>
-        <v>4.0999999999999996</v>
+        <v>5.45</v>
       </c>
       <c r="C33" s="9">
         <f>+C27</f>
@@ -1394,7 +1421,7 @@
       </c>
       <c r="B35" s="20">
         <f>+B24</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C35" s="11">
         <f>+C24+0.5</f>
@@ -1411,11 +1438,11 @@
       </c>
       <c r="B36" s="20">
         <f>+B25</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C36" s="11">
         <f>+C35+J9</f>
-        <v>2.9599999999999995</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D36" s="11">
         <f>+D25+0.5</f>
@@ -1428,11 +1455,11 @@
       </c>
       <c r="B37" s="20">
         <f>+B29</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C37" s="11">
         <f>+C35+$J$9</f>
-        <v>2.9599999999999995</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D37" s="11">
         <f>+D35+$K$9</f>
@@ -1445,7 +1472,7 @@
       </c>
       <c r="B38" s="20">
         <f>+B28</f>
-        <v>12</v>
+        <v>16.5</v>
       </c>
       <c r="C38" s="11">
         <f>+C28+0.5</f>
@@ -1462,11 +1489,11 @@
       </c>
       <c r="B39" s="21">
         <f>+B25-0.5</f>
-        <v>11.5</v>
+        <v>16</v>
       </c>
       <c r="C39" s="7">
         <f>+C25</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D39" s="7">
         <f>+D25+0.5</f>
@@ -1479,11 +1506,11 @@
       </c>
       <c r="B40" s="21">
         <f>+B39-$J$10</f>
-        <v>7.9</v>
+        <v>11.05</v>
       </c>
       <c r="C40" s="7">
         <f>+C26</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D40" s="7">
         <f>+D26+0.5</f>
@@ -1496,11 +1523,11 @@
       </c>
       <c r="B41" s="21">
         <f>+B40</f>
-        <v>7.9</v>
+        <v>11.05</v>
       </c>
       <c r="C41" s="7">
         <f>+C40</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D41" s="7">
         <f>+D40+$K$10</f>
@@ -1513,11 +1540,11 @@
       </c>
       <c r="B42" s="21">
         <f>+B39</f>
-        <v>11.5</v>
+        <v>16</v>
       </c>
       <c r="C42" s="7">
         <f>+C41</f>
-        <v>8.1999999999999993</v>
+        <v>12</v>
       </c>
       <c r="D42" s="7">
         <f>+D41</f>
@@ -1534,7 +1561,7 @@
       </c>
       <c r="C43" s="14">
         <f>+C26-0.5</f>
-        <v>7.6999999999999993</v>
+        <v>11.5</v>
       </c>
       <c r="D43" s="14">
         <f>+D26+0.5</f>
@@ -1551,7 +1578,7 @@
       </c>
       <c r="C44" s="14">
         <f>+C43-$J$11</f>
-        <v>5.24</v>
+        <v>7.9</v>
       </c>
       <c r="D44" s="14">
         <f>+D23+0.5</f>
@@ -1568,7 +1595,7 @@
       </c>
       <c r="C45" s="14">
         <f>+C44</f>
-        <v>5.24</v>
+        <v>7.9</v>
       </c>
       <c r="D45" s="14">
         <f>+D44+$K$11</f>
@@ -1585,7 +1612,7 @@
       </c>
       <c r="C46" s="14">
         <f>+C43</f>
-        <v>7.6999999999999993</v>
+        <v>11.5</v>
       </c>
       <c r="D46" s="14">
         <f>+D45</f>

</xml_diff>

<commit_message>
Updating the generic model. Some of the datapoints for the windows were incorrect. No impact on 3-storey model, just updating the spreadsheet.
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-3storey/3storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-3storey/3storey_model_geometry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19035" windowHeight="9210"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19230" windowHeight="5085"/>
   </bookViews>
   <sheets>
     <sheet name="geometry calculation" sheetId="1" r:id="rId1"/>
@@ -749,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,8 +1170,8 @@
         <v>82</v>
       </c>
       <c r="H17" s="24">
-        <f>3/12</f>
-        <v>0.25</v>
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
       </c>
       <c r="H18" s="23">
         <f>10.363+($C$3*H17)</f>
-        <v>14.488</v>
+        <v>13.113</v>
       </c>
       <c r="I18" s="13" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
adding multi-layer constructions to the retrofit.constrdb database.
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-3storey/3storey_model_geometry.xlsx
+++ b/OptFramework/GenericHome-3storey/3storey_model_geometry.xlsx
@@ -19,7 +19,7 @@
     <author>Purdy, Julia</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -49,14 +49,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="85">
   <si>
     <t>window geometry calculations</t>
   </si>
   <si>
-    <t>Floor Area</t>
-  </si>
-  <si>
     <t>window area ratio</t>
   </si>
   <si>
@@ -298,6 +295,15 @@
   </si>
   <si>
     <t>3/12</t>
+  </si>
+  <si>
+    <t>Total Floor Area</t>
+  </si>
+  <si>
+    <t>Floor Area per storey</t>
+  </si>
+  <si>
+    <t>number of storeys</t>
   </si>
 </sst>
 </file>
@@ -747,10 +753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,305 +778,309 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="13">
-        <f>+C3*C4</f>
-        <v>198</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>4</v>
+        <v>82</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>285.3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2">
-        <f>+(B24-B23)*(D29-D24)</f>
-        <v>50.291999999999994</v>
+        <f>+(B26-B25)*(D31-D26)</f>
+        <v>29.723860960514532</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="2">
-        <v>16.5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1"/>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3">
-        <f>+(C25-C24)*(D29-D25)</f>
-        <v>36.575999999999993</v>
+        <f>+(C27-C26)*(D31-D27)</f>
+        <v>29.723860960514532</v>
       </c>
       <c r="I3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" s="1">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>83</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13">
+        <f>+$C$2/C3</f>
+        <v>95.100000000000009</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>3</v>
+      </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4">
-        <f>+(B25-B26)*(D29-D26)</f>
-        <v>50.291999999999994</v>
+        <f>+(B27-B28)*(D31-D28)</f>
+        <v>29.723860960514532</v>
       </c>
       <c r="I4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="13">
-        <v>15</v>
-      </c>
-      <c r="D5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="2">
+        <f>+SQRT(C4)</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <f>+(C28-C25)*(D32-D28)</f>
+        <v>29.723860960514532</v>
+      </c>
+      <c r="I5" t="s">
         <v>3</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5">
-        <f>+(C26-C23)*(D30-D26)</f>
-        <v>36.575999999999993</v>
-      </c>
-      <c r="I5" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="13">
-        <v>2.4384000000000001</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="2">
+        <f>+SQRT(C4)</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1"/>
       <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6">
+        <f>+(B30*C31)</f>
+        <v>95.100000000000009</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
         <v>50</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>44</v>
       </c>
-      <c r="H6">
-        <f>+(B28*C29)</f>
-        <v>198</v>
-      </c>
-      <c r="I6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="13">
-        <v>2</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>45</v>
-      </c>
       <c r="H7">
-        <f>+C26*B25</f>
-        <v>198</v>
+        <f>+C28*B27</f>
+        <v>95.100000000000009</v>
       </c>
       <c r="I7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C8" s="13">
-        <f>3.048+C6</f>
-        <v>5.4863999999999997</v>
+        <v>2.4384000000000001</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H8" s="15">
-        <f>+H2*$C$5/100</f>
-        <v>7.5437999999999992</v>
+        <f>+H2*$C$7/100</f>
+        <v>4.4585791440771798</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J8" s="19">
         <f>+H8/K8</f>
-        <v>4.95</v>
+        <v>2.9255768661923756</v>
       </c>
       <c r="K8" s="9">
-        <f>+($C$8-$C$6)/2</f>
+        <f>+($C$10-$C$8)/2</f>
         <v>1.5239999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="13" t="s">
-        <v>78</v>
+      <c r="B9" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C9" s="13">
-        <f>+C3/2</f>
-        <v>8.25</v>
+        <v>2</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="16">
-        <f>+H3*$C$5/100</f>
-        <v>5.4863999999999988</v>
+        <f>+H3*$C$7/100</f>
+        <v>4.4585791440771798</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" s="20">
         <f t="shared" ref="J9" si="0">+H9/K9</f>
-        <v>3.5999999999999996</v>
+        <v>2.9255768661923756</v>
       </c>
       <c r="K9" s="11">
-        <f>+($C$8-$C$6)/2</f>
+        <f>+($C$10-$C$8)/2</f>
         <v>1.5239999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="8">
-        <f>+$D$32</f>
-        <v>2.9384000000000001</v>
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="13">
+        <f>3.048+C8</f>
+        <v>5.4863999999999997</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>6</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="17">
-        <f>+H4*$C$5/100</f>
-        <v>7.5437999999999992</v>
+        <f>+H4*$C$7/100</f>
+        <v>4.4585791440771798</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" s="21">
         <f>+H10/K10</f>
-        <v>4.95</v>
+        <v>2.9255768661923756</v>
       </c>
       <c r="K10" s="7">
-        <f t="shared" ref="K10:K11" si="1">+($C$8-$C$6)/2</f>
+        <f t="shared" ref="K10:K11" si="1">+($C$10-$C$8)/2</f>
         <v>1.5239999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="8">
-        <f>+$D$34</f>
-        <v>4.4623999999999997</v>
-      </c>
-      <c r="D11" s="1"/>
+      <c r="B11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="13">
+        <f>+C5/2</f>
+        <v>4.8759614436539591</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="F11" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" s="18">
-        <f>+H5*$C$5/100</f>
-        <v>5.4863999999999988</v>
+        <f>+H5*$C$7/100</f>
+        <v>4.4585791440771798</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J11" s="22">
         <f>+H11/K11</f>
-        <v>3.5999999999999996</v>
+        <v>2.9255768661923756</v>
       </c>
       <c r="K11" s="14">
         <f t="shared" si="1"/>
@@ -1078,25 +1088,24 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
       <c r="B12" s="8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12" s="8">
-        <f>+$B$31</f>
-        <v>0.5</v>
-      </c>
-      <c r="D12" s="1"/>
+        <f>+$D$34</f>
+        <v>2.9384000000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="15">
-        <f>+$B$32</f>
-        <v>5.45</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C13" s="8">
+        <f>+$D$36</f>
+        <v>4.4623999999999997</v>
+      </c>
+      <c r="D13" s="1"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="16"/>
@@ -1106,18 +1115,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="10">
-        <f>+$C$35</f>
+      <c r="B14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="8">
+        <f>+$B$33</f>
         <v>0.5</v>
       </c>
+      <c r="D14" s="1"/>
       <c r="F14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>80</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>81</v>
       </c>
       <c r="H14" s="24">
         <f>8/12</f>
@@ -1125,49 +1135,51 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="16">
-        <f>+$C$36</f>
-        <v>4.0999999999999996</v>
+      <c r="A15" s="1"/>
+      <c r="B15" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="15">
+        <f>+$B$34</f>
+        <v>3.4255768661923756</v>
       </c>
       <c r="F15" t="s">
+        <v>78</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="23">
+        <f>10.363+($C$5*H14)</f>
+        <v>16.864281924871946</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="10">
+        <f>+$C$37</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="16">
+        <f>+$C$38</f>
+        <v>3.4255768661923756</v>
+      </c>
+      <c r="F17" t="s">
         <v>79</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G17" s="25" t="s">
         <v>81</v>
-      </c>
-      <c r="H15" s="23">
-        <f>10.363+($C$3*H14)</f>
-        <v>21.363</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="17">
-        <f>+$B$39</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="17">
-        <f>+$B$40</f>
-        <v>11.05</v>
-      </c>
-      <c r="F17" t="s">
-        <v>80</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>82</v>
       </c>
       <c r="H17" s="24">
         <f>2/12</f>
@@ -1175,447 +1187,465 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="17">
+        <f>+$B$41</f>
+        <v>9.2519228873079182</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="23">
+        <f>10.363+($C$5*H17)</f>
+        <v>11.988320481217986</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="17">
+        <f>+$B$42</f>
+        <v>6.3263460211155422</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="12">
+        <f>+$C$45</f>
+        <v>9.2519228873079182</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="12">
-        <f>+$C$43</f>
-        <v>11.5</v>
-      </c>
-      <c r="F18" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="H18" s="23">
-        <f>10.363+($C$3*H17)</f>
-        <v>13.113</v>
-      </c>
-      <c r="I18" s="13" t="s">
+      <c r="C21" s="18">
+        <f>+$C$46</f>
+        <v>6.3263460211155422</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" s="18">
-        <f>+$C$44</f>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0</v>
-      </c>
-      <c r="D23" s="3">
-        <f>+$C$6</f>
-        <v>2.4384000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="4">
-        <f>+$C$3</f>
-        <v>16.5</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0</v>
-      </c>
-      <c r="D24" s="3">
-        <f>+$C$6</f>
-        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="4">
-        <f>+$C$3</f>
-        <v>16.5</v>
+        <v>12</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
       </c>
       <c r="C25" s="3">
-        <f>+$C$4</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D25" s="3">
-        <f>+$C$6</f>
+        <f>+$C$8</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="3">
+        <v>13</v>
+      </c>
+      <c r="B26" s="4">
+        <f>+$C$5</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="C26" s="3">
         <v>0</v>
       </c>
-      <c r="C26" s="3">
-        <f>+$C$4</f>
-        <v>12</v>
-      </c>
       <c r="D26" s="3">
-        <f>+$C$6</f>
+        <f>+$C$8</f>
         <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
-      </c>
-      <c r="B27" s="3">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="B27" s="4">
+        <f>+$C$5</f>
+        <v>9.7519228873079182</v>
       </c>
       <c r="C27" s="3">
-        <v>0</v>
+        <f>+$C$6</f>
+        <v>9.7519228873079182</v>
       </c>
       <c r="D27" s="3">
         <f>+$C$8</f>
-        <v>5.4863999999999997</v>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="4">
-        <f>+$C$3</f>
-        <v>16.5</v>
+        <v>15</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0</v>
       </c>
       <c r="C28" s="3">
-        <v>0</v>
+        <f>+$C$6</f>
+        <v>9.7519228873079182</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" ref="D28:D29" si="2">+$C$8</f>
-        <v>5.4863999999999997</v>
+        <f>+$C$8</f>
+        <v>2.4384000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>19</v>
-      </c>
-      <c r="B29" s="4">
-        <f>+$C$3</f>
-        <v>16.5</v>
+        <v>16</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0</v>
       </c>
       <c r="C29" s="3">
-        <f>+$C$4</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D29" s="3">
+        <f>+$C$10</f>
+        <v>5.4863999999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="4">
+        <f>+$C$5</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="C30" s="3">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" ref="D30:D31" si="2">+$C$10</f>
+        <v>5.4863999999999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="4">
+        <f>+$C$5</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="C31" s="3">
+        <f>+$C$6</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D31" s="3">
         <f t="shared" si="2"/>
         <v>5.4863999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="3">
         <v>0</v>
       </c>
-      <c r="C30" s="3">
-        <f>+$C$4</f>
-        <v>12</v>
-      </c>
-      <c r="D30" s="3">
-        <f>+$C$8</f>
+      <c r="C32" s="3">
+        <f>+$C$6</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D32" s="3">
+        <f>+$C$10</f>
         <v>5.4863999999999997</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="9">
-        <f>+B23+0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="C31" s="9">
-        <f>+C23</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="9">
-        <f>+$D$23+0.5</f>
-        <v>2.9384000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="19">
-        <f>+B31+$J$8</f>
-        <v>5.45</v>
-      </c>
-      <c r="C32" s="9">
-        <f>+C24</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="9">
-        <f>+$D$23+0.5</f>
-        <v>2.9384000000000001</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B33" s="19">
-        <f>+B31+$J$8</f>
-        <v>5.45</v>
+        <v>20</v>
+      </c>
+      <c r="B33" s="9">
+        <f>+B25+0.5</f>
+        <v>0.5</v>
       </c>
       <c r="C33" s="9">
-        <f>+C27</f>
+        <f>+C25</f>
         <v>0</v>
       </c>
       <c r="D33" s="9">
-        <f>+D31+$K$8</f>
-        <v>4.4623999999999997</v>
+        <f>+$D$25+0.5</f>
+        <v>2.9384000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="19">
+        <f>+B33+$J$8</f>
+        <v>3.4255768661923756</v>
+      </c>
+      <c r="C34" s="9">
+        <f>+C26</f>
+        <v>0</v>
+      </c>
+      <c r="D34" s="9">
+        <f>+$D$25+0.5</f>
+        <v>2.9384000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="19">
+        <f>+B33+$J$8</f>
+        <v>3.4255768661923756</v>
+      </c>
+      <c r="C35" s="9">
+        <f>+C29</f>
+        <v>0</v>
+      </c>
+      <c r="D35" s="9">
+        <f>+D33+$K$8</f>
+        <v>4.4623999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="9">
+        <f>+B33</f>
+        <v>0.5</v>
+      </c>
+      <c r="C36" s="9">
+        <f>+C30</f>
+        <v>0</v>
+      </c>
+      <c r="D36" s="9">
+        <f>+D34+$K$8</f>
+        <v>4.4623999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B37" s="20">
+        <f>+B26</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="C37" s="11">
+        <f>+C26+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="11">
+        <f>+D26+0.5</f>
+        <v>2.9384000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="20">
+        <f>+B27</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="C38" s="11">
+        <f>+C37+J9</f>
+        <v>3.4255768661923756</v>
+      </c>
+      <c r="D38" s="11">
+        <f>+D27+0.5</f>
+        <v>2.9384000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="20">
         <f>+B31</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="C39" s="11">
+        <f>+C37+$J$9</f>
+        <v>3.4255768661923756</v>
+      </c>
+      <c r="D39" s="11">
+        <f>+D37+$K$9</f>
+        <v>4.4623999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="20">
+        <f>+B30</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="C40" s="11">
+        <f>+C30+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="C34" s="9">
+      <c r="D40" s="11">
+        <f>+D38+$K$9</f>
+        <v>4.4623999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="21">
+        <f>+B27-0.5</f>
+        <v>9.2519228873079182</v>
+      </c>
+      <c r="C41" s="7">
+        <f>+C27</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D41" s="7">
+        <f>+D27+0.5</f>
+        <v>2.9384000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" s="21">
+        <f>+B41-$J$10</f>
+        <v>6.3263460211155422</v>
+      </c>
+      <c r="C42" s="7">
         <f>+C28</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D42" s="7">
+        <f>+D28+0.5</f>
+        <v>2.9384000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" s="21">
+        <f>+B42</f>
+        <v>6.3263460211155422</v>
+      </c>
+      <c r="C43" s="7">
+        <f>+C42</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D43" s="7">
+        <f>+D42+$K$10</f>
+        <v>4.4623999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" s="21">
+        <f>+B41</f>
+        <v>9.2519228873079182</v>
+      </c>
+      <c r="C44" s="7">
+        <f>+C43</f>
+        <v>9.7519228873079182</v>
+      </c>
+      <c r="D44" s="7">
+        <f>+D43</f>
+        <v>4.4623999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="14">
+        <f>+B28</f>
         <v>0</v>
       </c>
-      <c r="D34" s="9">
-        <f>+D32+$K$8</f>
-        <v>4.4623999999999997</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B35" s="20">
-        <f>+B24</f>
-        <v>16.5</v>
-      </c>
-      <c r="C35" s="11">
-        <f>+C24+0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="D35" s="11">
-        <f>+D24+0.5</f>
+      <c r="C45" s="14">
+        <f>+C28-0.5</f>
+        <v>9.2519228873079182</v>
+      </c>
+      <c r="D45" s="14">
+        <f>+D28+0.5</f>
         <v>2.9384000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" s="20">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="14">
         <f>+B25</f>
-        <v>16.5</v>
-      </c>
-      <c r="C36" s="11">
-        <f>+C35+J9</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D36" s="11">
+        <v>0</v>
+      </c>
+      <c r="C46" s="14">
+        <f>+C45-$J$11</f>
+        <v>6.3263460211155422</v>
+      </c>
+      <c r="D46" s="14">
         <f>+D25+0.5</f>
         <v>2.9384000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" s="20">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="14">
         <f>+B29</f>
-        <v>16.5</v>
-      </c>
-      <c r="C37" s="11">
-        <f>+C35+$J$9</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D37" s="11">
-        <f>+D35+$K$9</f>
+        <v>0</v>
+      </c>
+      <c r="C47" s="14">
+        <f>+C46</f>
+        <v>6.3263460211155422</v>
+      </c>
+      <c r="D47" s="14">
+        <f>+D46+$K$11</f>
         <v>4.4623999999999997</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="20">
-        <f>+B28</f>
-        <v>16.5</v>
-      </c>
-      <c r="C38" s="11">
-        <f>+C28+0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="D38" s="11">
-        <f>+D36+$K$9</f>
-        <v>4.4623999999999997</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="21">
-        <f>+B25-0.5</f>
-        <v>16</v>
-      </c>
-      <c r="C39" s="7">
-        <f>+C25</f>
-        <v>12</v>
-      </c>
-      <c r="D39" s="7">
-        <f>+D25+0.5</f>
-        <v>2.9384000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="21">
-        <f>+B39-$J$10</f>
-        <v>11.05</v>
-      </c>
-      <c r="C40" s="7">
-        <f>+C26</f>
-        <v>12</v>
-      </c>
-      <c r="D40" s="7">
-        <f>+D26+0.5</f>
-        <v>2.9384000000000001</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="21">
-        <f>+B40</f>
-        <v>11.05</v>
-      </c>
-      <c r="C41" s="7">
-        <f>+C40</f>
-        <v>12</v>
-      </c>
-      <c r="D41" s="7">
-        <f>+D40+$K$10</f>
-        <v>4.4623999999999997</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="21">
-        <f>+B39</f>
-        <v>16</v>
-      </c>
-      <c r="C42" s="7">
-        <f>+C41</f>
-        <v>12</v>
-      </c>
-      <c r="D42" s="7">
-        <f>+D41</f>
-        <v>4.4623999999999997</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" s="14">
-        <f>+B26</f>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="14">
+        <f>+B32</f>
         <v>0</v>
       </c>
-      <c r="C43" s="14">
-        <f>+C26-0.5</f>
-        <v>11.5</v>
-      </c>
-      <c r="D43" s="14">
-        <f>+D26+0.5</f>
-        <v>2.9384000000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B44" s="14">
-        <f>+B23</f>
-        <v>0</v>
-      </c>
-      <c r="C44" s="14">
-        <f>+C43-$J$11</f>
-        <v>7.9</v>
-      </c>
-      <c r="D44" s="14">
-        <f>+D23+0.5</f>
-        <v>2.9384000000000001</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="14">
-        <f>+B27</f>
-        <v>0</v>
-      </c>
-      <c r="C45" s="14">
-        <f>+C44</f>
-        <v>7.9</v>
-      </c>
-      <c r="D45" s="14">
-        <f>+D44+$K$11</f>
-        <v>4.4623999999999997</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B46" s="14">
-        <f>+B30</f>
-        <v>0</v>
-      </c>
-      <c r="C46" s="14">
-        <f>+C43</f>
-        <v>11.5</v>
-      </c>
-      <c r="D46" s="14">
-        <f>+D45</f>
+      <c r="C48" s="14">
+        <f>+C45</f>
+        <v>9.2519228873079182</v>
+      </c>
+      <c r="D48" s="14">
+        <f>+D47</f>
         <v>4.4623999999999997</v>
       </c>
     </row>

</xml_diff>